<commit_message>
Angular 2 - Pluralsight videos
</commit_message>
<xml_diff>
--- a/To-do.xlsx
+++ b/To-do.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="384">
   <si>
     <t>Junit + Spring + Mockito + Powermock</t>
   </si>
@@ -1172,6 +1172,24 @@
   </si>
   <si>
     <t>AngularJS Application Development [Course]</t>
+  </si>
+  <si>
+    <t>Angular Fundamentals</t>
+  </si>
+  <si>
+    <t>Angular: First Look</t>
+  </si>
+  <si>
+    <t>Building Components with Angular 1.5</t>
+  </si>
+  <si>
+    <t>Angular 1.x</t>
+  </si>
+  <si>
+    <t>Angular 2</t>
+  </si>
+  <si>
+    <t>Angular: Getting Started [Course]</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1244,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1266,6 +1284,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,7 +1356,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1420,6 +1444,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1447,6 +1472,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1457,8 +1485,8 @@
   <colors>
     <mruColors>
       <color rgb="FF33CC33"/>
+      <color rgb="FF0000CC"/>
       <color rgb="FF3302BE"/>
-      <color rgb="FF0000CC"/>
       <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
@@ -2356,11 +2384,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2376,48 +2404,46 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="59"/>
+    </row>
+    <row r="3" spans="1:2" s="48" customFormat="1">
+      <c r="A3" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B6" s="45" t="s">
+    <row r="5" spans="1:2" s="48" customFormat="1">
+      <c r="A5" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="48" customFormat="1">
+      <c r="A6" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B7" s="45" t="s">
         <v>11</v>
@@ -2425,7 +2451,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B8" s="45" t="s">
         <v>11</v>
@@ -2433,7 +2459,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B9" s="45" t="s">
         <v>11</v>
@@ -2441,7 +2467,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>11</v>
@@ -2449,7 +2475,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B11" s="45" t="s">
         <v>11</v>
@@ -2457,7 +2483,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B12" s="45" t="s">
         <v>11</v>
@@ -2465,7 +2491,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B13" s="45" t="s">
         <v>11</v>
@@ -2473,31 +2499,85 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B17" s="45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="59" t="s">
+        <v>382</v>
+      </c>
+      <c r="B21" s="59"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B22" s="48" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" display="https://app.pluralsight.com/library/courses/angularjs-security-fundamentals"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://app.pluralsight.com/library/courses/angular-big-picture"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://app.pluralsight.com/library/courses/angularjs-get-started"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://app.pluralsight.com/library/courses/angularjs-ngmock-unit-testing"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://app.pluralsight.com/library/courses/angularjs-services-in-depth"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://app.pluralsight.com/library/courses/angular-routing-in-depth"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://app.pluralsight.com/library/courses/angularjs-patterns-clean-code"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://app.pluralsight.com/library/courses/angularjs-in-depth"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://app.pluralsight.com/library/courses/angular-web-api-front-back"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://app.pluralsight.com/library/courses/angularjs-forms-bootstrap-mvc5"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://app.pluralsight.com/library/courses/angularjs-directive-fundamentals"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://app.pluralsight.com/library/courses/angular-best-practices"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://app.pluralsight.com/library/courses/angular-application-development"/>
+    <hyperlink ref="A17" r:id="rId1" display="https://app.pluralsight.com/library/courses/angularjs-security-fundamentals"/>
+    <hyperlink ref="A4" r:id="rId2" display="https://app.pluralsight.com/library/courses/angularjs-get-started"/>
+    <hyperlink ref="A7" r:id="rId3" display="https://app.pluralsight.com/library/courses/angularjs-ngmock-unit-testing"/>
+    <hyperlink ref="A8" r:id="rId4" display="https://app.pluralsight.com/library/courses/angularjs-services-in-depth"/>
+    <hyperlink ref="A9" r:id="rId5" display="https://app.pluralsight.com/library/courses/angular-routing-in-depth"/>
+    <hyperlink ref="A10" r:id="rId6" display="https://app.pluralsight.com/library/courses/angularjs-patterns-clean-code"/>
+    <hyperlink ref="A11" r:id="rId7" display="https://app.pluralsight.com/library/courses/angularjs-in-depth"/>
+    <hyperlink ref="A12" r:id="rId8" display="https://app.pluralsight.com/library/courses/angular-web-api-front-back"/>
+    <hyperlink ref="A13" r:id="rId9" display="https://app.pluralsight.com/library/courses/angularjs-forms-bootstrap-mvc5"/>
+    <hyperlink ref="A14" r:id="rId10" display="https://app.pluralsight.com/library/courses/angularjs-directive-fundamentals"/>
+    <hyperlink ref="A15" r:id="rId11" display="https://app.pluralsight.com/library/courses/angular-best-practices"/>
+    <hyperlink ref="A16" r:id="rId12" display="https://app.pluralsight.com/library/courses/angular-application-development"/>
     <hyperlink ref="A1" location="Topics!A16" display="Topics"/>
+    <hyperlink ref="A5" r:id="rId13" tooltip="Angular Fundamentals" display="https://app.pluralsight.com/library/courses/angularjs-fundamentals"/>
+    <hyperlink ref="A6" r:id="rId14" tooltip="Angular: First Look" display="https://app.pluralsight.com/library/courses/angular-2-first-look"/>
+    <hyperlink ref="A18" r:id="rId15" tooltip="Building Components with Angular 1.5" display="https://app.pluralsight.com/library/courses/building-components-angular-1-5"/>
+    <hyperlink ref="A3" r:id="rId16" display="https://app.pluralsight.com/library/courses/angular-big-picture"/>
+    <hyperlink ref="A22" r:id="rId17" display="https://app.pluralsight.com/library/courses/angular-2-getting-started-update"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -3146,10 +3226,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="53"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
@@ -3188,10 +3268,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="53"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
@@ -3403,7 +3483,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="50" t="s">
         <v>113</v>
       </c>
       <c r="B13" t="s">
@@ -3411,7 +3491,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -3432,7 +3512,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="50" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -3443,13 +3523,13 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="49"/>
+      <c r="A19" s="50"/>
       <c r="B19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
@@ -3458,7 +3538,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
@@ -3467,13 +3547,13 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="50" t="s">
         <v>114</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -3484,37 +3564,37 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="49"/>
+      <c r="A28" s="50"/>
       <c r="B28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="49"/>
+      <c r="A29" s="50"/>
       <c r="B29" t="s">
         <v>47</v>
       </c>
@@ -3525,7 +3605,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="50" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -3536,43 +3616,43 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="49"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="49"/>
+      <c r="A33" s="50"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="49"/>
+      <c r="A34" s="50"/>
       <c r="B34" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="49"/>
+      <c r="A35" s="50"/>
       <c r="B35" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="49"/>
+      <c r="A36" s="50"/>
       <c r="B36" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="49"/>
+      <c r="A37" s="50"/>
       <c r="B37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="50" t="s">
         <v>55</v>
       </c>
       <c r="B38" t="s">
@@ -3580,19 +3660,19 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="49"/>
+      <c r="A39" s="50"/>
       <c r="B39" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="49"/>
+      <c r="A40" s="50"/>
       <c r="B40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="50" t="s">
         <v>56</v>
       </c>
       <c r="B41" t="s">
@@ -3600,25 +3680,25 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="49"/>
+      <c r="A42" s="50"/>
       <c r="B42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="49"/>
+      <c r="A43" s="50"/>
       <c r="B43" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="49"/>
+      <c r="A44" s="50"/>
       <c r="B44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="50" t="s">
         <v>91</v>
       </c>
       <c r="B45" t="s">
@@ -3626,7 +3706,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="49"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="10" t="s">
         <v>67</v>
       </c>
@@ -3635,7 +3715,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="49"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="10" t="s">
         <v>68</v>
       </c>
@@ -3659,7 +3739,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="50" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -3670,13 +3750,13 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="49"/>
+      <c r="A52" s="50"/>
       <c r="B52" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="49"/>
+      <c r="A53" s="50"/>
       <c r="B53" t="s">
         <v>78</v>
       </c>
@@ -3692,7 +3772,7 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B56" t="s">
@@ -3700,13 +3780,13 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="49"/>
+      <c r="A57" s="50"/>
       <c r="B57" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="49" t="s">
+      <c r="A58" s="50" t="s">
         <v>103</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -3717,7 +3797,7 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="49"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="10" t="s">
         <v>104</v>
       </c>
@@ -3726,7 +3806,7 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="49"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="10" t="s">
         <v>105</v>
       </c>
@@ -3735,7 +3815,7 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="50" t="s">
         <v>83</v>
       </c>
       <c r="B61" t="s">
@@ -3743,31 +3823,31 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="49"/>
+      <c r="A62" s="50"/>
       <c r="B62" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="49"/>
+      <c r="A63" s="50"/>
       <c r="B63" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="49"/>
+      <c r="A64" s="50"/>
       <c r="B64" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="49"/>
+      <c r="A65" s="50"/>
       <c r="B65" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="49"/>
+      <c r="A66" s="50"/>
       <c r="B66" t="s">
         <v>101</v>
       </c>
@@ -3778,7 +3858,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="50" t="s">
+      <c r="A68" s="51" t="s">
         <v>87</v>
       </c>
       <c r="B68" t="s">
@@ -3786,55 +3866,55 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="50"/>
+      <c r="A69" s="51"/>
       <c r="B69" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="50"/>
+      <c r="A70" s="51"/>
       <c r="B70" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="50"/>
+      <c r="A71" s="51"/>
       <c r="B71" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="50"/>
+      <c r="A72" s="51"/>
       <c r="B72" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="50"/>
+      <c r="A73" s="51"/>
       <c r="B73" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="50"/>
+      <c r="A74" s="51"/>
       <c r="B74" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="50"/>
+      <c r="A75" s="51"/>
       <c r="B75" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="50"/>
+      <c r="A76" s="51"/>
       <c r="B76" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="50"/>
+      <c r="A77" s="51"/>
       <c r="B77" s="10" t="s">
         <v>85</v>
       </c>
@@ -3863,7 +3943,7 @@
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="49" t="s">
+      <c r="A82" s="50" t="s">
         <v>109</v>
       </c>
       <c r="B82" s="10" t="s">
@@ -3871,49 +3951,49 @@
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="49"/>
+      <c r="A83" s="50"/>
       <c r="B83" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="49"/>
+      <c r="A84" s="50"/>
       <c r="B84" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="49"/>
+      <c r="A85" s="50"/>
       <c r="B85" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="49"/>
+      <c r="A86" s="50"/>
       <c r="B86" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="49"/>
+      <c r="A87" s="50"/>
       <c r="B87" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="49"/>
+      <c r="A88" s="50"/>
       <c r="B88" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="49"/>
+      <c r="A89" s="50"/>
       <c r="B89" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="49"/>
+      <c r="A90" s="50"/>
       <c r="B90" t="s">
         <v>133</v>
       </c>
@@ -3934,7 +4014,7 @@
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="48" t="s">
+      <c r="A94" s="49" t="s">
         <v>155</v>
       </c>
       <c r="B94" s="10" t="s">
@@ -3942,7 +4022,7 @@
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="48"/>
+      <c r="A95" s="49"/>
       <c r="B95" t="s">
         <v>157</v>
       </c>
@@ -3990,10 +4070,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
@@ -4004,10 +4084,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="52" t="s">
         <v>330</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="53"/>
     </row>
     <row r="5" spans="1:6" s="36" customFormat="1">
       <c r="A5" s="18" t="s">
@@ -4034,14 +4114,14 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="34" t="s">
@@ -4054,14 +4134,14 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24" t="s">
@@ -4085,14 +4165,14 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="28" t="s">
@@ -4108,14 +4188,14 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="54" t="s">
         <v>328</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="22" t="s">
@@ -4143,10 +4223,10 @@
       <c r="B22" s="28"/>
     </row>
     <row r="23" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="52"/>
+      <c r="B23" s="53"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="24" t="s">
@@ -4158,10 +4238,10 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="52"/>
+      <c r="B26" s="53"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
@@ -4194,10 +4274,10 @@
     </row>
     <row r="31" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="32" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="52" t="s">
         <v>329</v>
       </c>
-      <c r="B32" s="52"/>
+      <c r="B32" s="53"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="24" t="s">
@@ -4229,10 +4309,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="52"/>
+      <c r="B37" s="53"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
@@ -4598,11 +4678,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
@@ -4693,11 +4773,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="31" t="s">

</xml_diff>

<commit_message>
Javascript - Pluralsight videos list
</commit_message>
<xml_diff>
--- a/To-do.xlsx
+++ b/To-do.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="987" firstSheet="1" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="987" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="5" r:id="rId1"/>
@@ -32,13 +32,14 @@
     <sheet name="JMS" sheetId="25" r:id="rId23"/>
     <sheet name="npm" sheetId="26" r:id="rId24"/>
     <sheet name="git" sheetId="27" r:id="rId25"/>
+    <sheet name="JS" sheetId="28" r:id="rId26"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="400">
   <si>
     <t>Junit + Spring + Mockito + Powermock</t>
   </si>
@@ -1190,6 +1191,54 @@
   </si>
   <si>
     <t>Angular: Getting Started [Course]</t>
+  </si>
+  <si>
+    <t>Basics of Programming with JavaScript</t>
+  </si>
+  <si>
+    <t>Building a JavaScript Development Environment</t>
+  </si>
+  <si>
+    <t>Front-End Web Development Quick Start With HTML5, CSS, and JavaScript</t>
+  </si>
+  <si>
+    <t>Advanced JavaScript</t>
+  </si>
+  <si>
+    <t>Practical Design Patterns in JavaScript</t>
+  </si>
+  <si>
+    <t>Quick Start to JavaScript: Volume 1</t>
+  </si>
+  <si>
+    <t>Rapid JavaScript Training</t>
+  </si>
+  <si>
+    <t>JavaScript: From Fundamentals to Functional JS</t>
+  </si>
+  <si>
+    <t>JavaScript Objects and Prototypes</t>
+  </si>
+  <si>
+    <t>D3.js Data Visualization Fundamentals</t>
+  </si>
+  <si>
+    <t>JavaScript Best Practices</t>
+  </si>
+  <si>
+    <t>JavaScript From Scratch</t>
+  </si>
+  <si>
+    <t>JavaScript: Advanced Fundamentals to jQuery &amp; Pure DOM Scripting</t>
+  </si>
+  <si>
+    <t>JavaScript Fundamentals</t>
+  </si>
+  <si>
+    <t>Quick Start to JavaScript: Volume 2</t>
+  </si>
+  <si>
+    <t>JavaScript: The Good Parts</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1831,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1933,7 +1982,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="40" t="s">
@@ -1965,6 +2014,7 @@
     <hyperlink ref="A22" location="WS!A1" display="Web Services(WS)"/>
     <hyperlink ref="A26" location="npm!A1" display="npm"/>
     <hyperlink ref="A27" location="git!A1" display="git"/>
+    <hyperlink ref="A28" location="JS!A1" display="Javascript"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2106,7 +2156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2386,9 +2436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3400,6 +3450,131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="115.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1">
+      <c r="A1" s="21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="18" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="18" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="18" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="18" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="18" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="18" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="18" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="18" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="18" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="18" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="18" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="18" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="18" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="18" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Topics!A28" display="Topics"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="Basics of Programming with JavaScript" display="https://app.pluralsight.com/library/courses/javascript-programming-basics"/>
+    <hyperlink ref="A3" r:id="rId2" tooltip="Building a JavaScript Development Environment" display="https://app.pluralsight.com/library/courses/javascript-development-environment"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="Front-End Web Development Quick Start With HTML5, CSS, and JavaScript" display="https://app.pluralsight.com/library/courses/front-end-web-app-html5-javascript-css"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="Advanced JavaScript" display="https://app.pluralsight.com/library/courses/advanced-javascript"/>
+    <hyperlink ref="A6" r:id="rId5" tooltip="Practical Design Patterns in JavaScript" display="https://app.pluralsight.com/library/courses/javascript-practical-design-patterns"/>
+    <hyperlink ref="A7" r:id="rId6" tooltip="Quick Start to JavaScript: Volume 1" display="https://app.pluralsight.com/library/courses/quick-start-javascript-1-1870"/>
+    <hyperlink ref="A8" r:id="rId7" tooltip="Rapid JavaScript Training" display="https://app.pluralsight.com/library/courses/rapid-javascript-training"/>
+    <hyperlink ref="A9" r:id="rId8" tooltip="JavaScript: From Fundamentals to Functional JS" display="https://app.pluralsight.com/library/courses/javascript-from-fundamentals-to-functional-js"/>
+    <hyperlink ref="A10" r:id="rId9" tooltip="JavaScript Objects and Prototypes" display="https://app.pluralsight.com/library/courses/javascript-objects-prototypes"/>
+    <hyperlink ref="A11" r:id="rId10" tooltip="D3.js Data Visualization Fundamentals" display="https://app.pluralsight.com/library/courses/d3js-data-visualization-fundamentals"/>
+    <hyperlink ref="A12" r:id="rId11" tooltip="JavaScript Best Practices" display="https://app.pluralsight.com/library/courses/javascript-best-practices"/>
+    <hyperlink ref="A13" r:id="rId12" tooltip="JavaScript From Scratch" display="https://app.pluralsight.com/library/courses/javascript-from-scratch"/>
+    <hyperlink ref="A14" r:id="rId13" tooltip="JavaScript: Advanced Fundamentals to jQuery &amp; Pure DOM Scripting" display="https://app.pluralsight.com/library/courses/advanced-js-jquery-pure-dom-scripting-fundamentals"/>
+    <hyperlink ref="A15" r:id="rId14" tooltip="JavaScript Fundamentals" display="https://app.pluralsight.com/library/courses/jscript-fundamentals"/>
+    <hyperlink ref="A16" r:id="rId15" tooltip="Quick Start to JavaScript: Volume 2" display="https://app.pluralsight.com/library/courses/quick-start-javascript-2-1917"/>
+    <hyperlink ref="A17" r:id="rId16" tooltip="JavaScript: The Good Parts" display="https://app.pluralsight.com/library/courses/javascript-good-parts"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C95"/>

</xml_diff>

<commit_message>
AngularJS:Get Started - completed
</commit_message>
<xml_diff>
--- a/To-do.xlsx
+++ b/To-do.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="987" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="987" firstSheet="2" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="5" r:id="rId1"/>
@@ -33,13 +33,14 @@
     <sheet name="npm" sheetId="26" r:id="rId24"/>
     <sheet name="git" sheetId="27" r:id="rId25"/>
     <sheet name="JS" sheetId="28" r:id="rId26"/>
+    <sheet name="BC" sheetId="29" r:id="rId27"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="405">
   <si>
     <t>Junit + Spring + Mockito + Powermock</t>
   </si>
@@ -1239,6 +1240,21 @@
   </si>
   <si>
     <t>JavaScript: The Good Parts</t>
+  </si>
+  <si>
+    <t>RESTful Web Services with Node.js and Express [Course]</t>
+  </si>
+  <si>
+    <t>Node.js and the Internet of Things Using Intel Edison [Course]</t>
+  </si>
+  <si>
+    <t>Block Chain(BC)</t>
+  </si>
+  <si>
+    <t>Blockchain Fundamentals</t>
+  </si>
+  <si>
+    <t>An AngularJS Playbook</t>
   </si>
 </sst>
 </file>
@@ -1405,7 +1421,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1494,6 +1510,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1522,6 +1539,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1827,11 +1853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1987,6 +2013,11 @@
       </c>
       <c r="B28" s="40" t="s">
         <v>361</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -2015,6 +2046,7 @@
     <hyperlink ref="A26" location="npm!A1" display="npm"/>
     <hyperlink ref="A27" location="git!A1" display="git"/>
     <hyperlink ref="A28" location="JS!A1" display="Javascript"/>
+    <hyperlink ref="A29" location="BC!A1" display="Block Chain(BC)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2154,9 +2186,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2191,14 +2223,27 @@
         <v>310</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://app.pluralsight.com/library/courses/node-intro"/>
     <hyperlink ref="A4" r:id="rId2" display="https://app.pluralsight.com/library/courses/full-stack-nodejs"/>
     <hyperlink ref="A3" r:id="rId3" display="https://app.pluralsight.com/library/courses/nodejs-advanced"/>
     <hyperlink ref="A1" location="Topics!A11" display="Topics"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://app.pluralsight.com/library/courses/node-js-express-rest-web-services"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://app.pluralsight.com/library/courses/nodejs-internet-of-things-intel-edison"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2436,9 +2481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2448,16 +2493,17 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="45" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" s="45" customFormat="1">
+      <c r="A1" s="63" t="s">
         <v>297</v>
       </c>
+      <c r="B1" s="63"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="B2" s="59"/>
+      <c r="B2" s="60"/>
     </row>
     <row r="3" spans="1:2" s="48" customFormat="1">
       <c r="A3" s="22" t="s">
@@ -2468,10 +2514,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2587,11 +2633,16 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="18" t="s">
+        <v>404</v>
+      </c>
+    </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="60" t="s">
         <v>382</v>
       </c>
-      <c r="B21" s="59"/>
+      <c r="B21" s="60"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
@@ -2602,9 +2653,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A17" r:id="rId1" display="https://app.pluralsight.com/library/courses/angularjs-security-fundamentals"/>
@@ -2625,9 +2677,10 @@
     <hyperlink ref="A18" r:id="rId15" tooltip="Building Components with Angular 1.5" display="https://app.pluralsight.com/library/courses/building-components-angular-1-5"/>
     <hyperlink ref="A3" r:id="rId16" display="https://app.pluralsight.com/library/courses/angular-big-picture"/>
     <hyperlink ref="A22" r:id="rId17" display="https://app.pluralsight.com/library/courses/angular-2-getting-started-update"/>
+    <hyperlink ref="A19" r:id="rId18" tooltip="An AngularJS Playbook" display="https://app.pluralsight.com/library/courses/angularjs-playbook"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -3276,10 +3329,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
@@ -3318,10 +3371,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
@@ -3452,11 +3505,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3465,89 +3518,137 @@
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
       <c r="A1" s="21" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="18" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="18" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="18" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="18" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="18" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="18" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="18" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="18" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="18" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="18" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="18" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="18" t="s">
         <v>399</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3575,6 +3676,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="109.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A1" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="62"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Topics!A29" display="Topics"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="Blockchain Fundamentals" display="https://app.pluralsight.com/library/courses/blockchain-fundamentals"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C95"/>
@@ -3658,7 +3799,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="51" t="s">
         <v>113</v>
       </c>
       <c r="B13" t="s">
@@ -3666,7 +3807,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -3687,7 +3828,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="51" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -3698,13 +3839,13 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="50"/>
+      <c r="A19" s="51"/>
       <c r="B19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="50"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
@@ -3713,7 +3854,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="50"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
@@ -3722,13 +3863,13 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="50"/>
+      <c r="A22" s="51"/>
       <c r="B22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="51" t="s">
         <v>114</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -3739,37 +3880,37 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="50"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="50"/>
+      <c r="A25" s="51"/>
       <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="50"/>
+      <c r="A26" s="51"/>
       <c r="B26" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="50"/>
+      <c r="A27" s="51"/>
       <c r="B27" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="50"/>
+      <c r="A28" s="51"/>
       <c r="B28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" t="s">
         <v>47</v>
       </c>
@@ -3780,7 +3921,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="51" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -3791,43 +3932,43 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="50"/>
+      <c r="A32" s="51"/>
       <c r="B32" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="50"/>
+      <c r="A33" s="51"/>
       <c r="B33" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="50"/>
+      <c r="A34" s="51"/>
       <c r="B34" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="50"/>
+      <c r="A35" s="51"/>
       <c r="B35" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="50"/>
+      <c r="A36" s="51"/>
       <c r="B36" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="50"/>
+      <c r="A37" s="51"/>
       <c r="B37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="51" t="s">
         <v>55</v>
       </c>
       <c r="B38" t="s">
@@ -3835,19 +3976,19 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="50"/>
+      <c r="A39" s="51"/>
       <c r="B39" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="51" t="s">
         <v>56</v>
       </c>
       <c r="B41" t="s">
@@ -3855,25 +3996,25 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="50"/>
+      <c r="A42" s="51"/>
       <c r="B42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="50"/>
+      <c r="A43" s="51"/>
       <c r="B43" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="50"/>
+      <c r="A44" s="51"/>
       <c r="B44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="50" t="s">
+      <c r="A45" s="51" t="s">
         <v>91</v>
       </c>
       <c r="B45" t="s">
@@ -3881,7 +4022,7 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="50"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="10" t="s">
         <v>67</v>
       </c>
@@ -3890,7 +4031,7 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="50"/>
+      <c r="A47" s="51"/>
       <c r="B47" s="10" t="s">
         <v>68</v>
       </c>
@@ -3914,7 +4055,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="50" t="s">
+      <c r="A51" s="51" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -3925,13 +4066,13 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="50"/>
+      <c r="A52" s="51"/>
       <c r="B52" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="50"/>
+      <c r="A53" s="51"/>
       <c r="B53" t="s">
         <v>78</v>
       </c>
@@ -3947,7 +4088,7 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="50" t="s">
+      <c r="A56" s="51" t="s">
         <v>107</v>
       </c>
       <c r="B56" t="s">
@@ -3955,13 +4096,13 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="50"/>
+      <c r="A57" s="51"/>
       <c r="B57" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="50" t="s">
+      <c r="A58" s="51" t="s">
         <v>103</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -3972,7 +4113,7 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="50"/>
+      <c r="A59" s="51"/>
       <c r="B59" s="10" t="s">
         <v>104</v>
       </c>
@@ -3981,7 +4122,7 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="50"/>
+      <c r="A60" s="51"/>
       <c r="B60" s="10" t="s">
         <v>105</v>
       </c>
@@ -3990,7 +4131,7 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="50" t="s">
+      <c r="A61" s="51" t="s">
         <v>83</v>
       </c>
       <c r="B61" t="s">
@@ -3998,31 +4139,31 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="50"/>
+      <c r="A62" s="51"/>
       <c r="B62" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="50"/>
+      <c r="A63" s="51"/>
       <c r="B63" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="50"/>
+      <c r="A64" s="51"/>
       <c r="B64" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="50"/>
+      <c r="A65" s="51"/>
       <c r="B65" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="50"/>
+      <c r="A66" s="51"/>
       <c r="B66" t="s">
         <v>101</v>
       </c>
@@ -4033,7 +4174,7 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="51" t="s">
+      <c r="A68" s="52" t="s">
         <v>87</v>
       </c>
       <c r="B68" t="s">
@@ -4041,55 +4182,55 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="51"/>
+      <c r="A69" s="52"/>
       <c r="B69" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="51"/>
+      <c r="A70" s="52"/>
       <c r="B70" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="51"/>
+      <c r="A71" s="52"/>
       <c r="B71" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="51"/>
+      <c r="A72" s="52"/>
       <c r="B72" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="51"/>
+      <c r="A73" s="52"/>
       <c r="B73" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="51"/>
+      <c r="A74" s="52"/>
       <c r="B74" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="51"/>
+      <c r="A75" s="52"/>
       <c r="B75" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="51"/>
+      <c r="A76" s="52"/>
       <c r="B76" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="51"/>
+      <c r="A77" s="52"/>
       <c r="B77" s="10" t="s">
         <v>85</v>
       </c>
@@ -4118,7 +4259,7 @@
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="50" t="s">
+      <c r="A82" s="51" t="s">
         <v>109</v>
       </c>
       <c r="B82" s="10" t="s">
@@ -4126,49 +4267,49 @@
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="50"/>
+      <c r="A83" s="51"/>
       <c r="B83" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="50"/>
+      <c r="A84" s="51"/>
       <c r="B84" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="50"/>
+      <c r="A85" s="51"/>
       <c r="B85" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="50"/>
+      <c r="A86" s="51"/>
       <c r="B86" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="50"/>
+      <c r="A87" s="51"/>
       <c r="B87" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="50"/>
+      <c r="A88" s="51"/>
       <c r="B88" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="50"/>
+      <c r="A89" s="51"/>
       <c r="B89" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="50"/>
+      <c r="A90" s="51"/>
       <c r="B90" t="s">
         <v>133</v>
       </c>
@@ -4189,7 +4330,7 @@
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="49" t="s">
+      <c r="A94" s="50" t="s">
         <v>155</v>
       </c>
       <c r="B94" s="10" t="s">
@@ -4197,7 +4338,7 @@
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="49"/>
+      <c r="A95" s="50"/>
       <c r="B95" t="s">
         <v>157</v>
       </c>
@@ -4245,10 +4386,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
@@ -4259,10 +4400,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>330</v>
       </c>
-      <c r="B4" s="53"/>
+      <c r="B4" s="54"/>
     </row>
     <row r="5" spans="1:6" s="36" customFormat="1">
       <c r="A5" s="18" t="s">
@@ -4289,14 +4430,14 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="34" t="s">
@@ -4309,14 +4450,14 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24" t="s">
@@ -4340,14 +4481,14 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="28" t="s">
@@ -4363,14 +4504,14 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>328</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="22" t="s">
@@ -4398,10 +4539,10 @@
       <c r="B22" s="28"/>
     </row>
     <row r="23" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="53"/>
+      <c r="B23" s="54"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="24" t="s">
@@ -4413,10 +4554,10 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="53"/>
+      <c r="B26" s="54"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
@@ -4449,10 +4590,10 @@
     </row>
     <row r="31" spans="1:6" s="28" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="32" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="54"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="24" t="s">
@@ -4484,10 +4625,10 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="53" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="53"/>
+      <c r="B37" s="54"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
@@ -4853,11 +4994,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="16" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
@@ -4948,11 +5089,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="31" t="s">

</xml_diff>

<commit_message>
1. Renamed Apache Camel folder 2. Multithreading 3. Todo
</commit_message>
<xml_diff>
--- a/To-do.xlsx
+++ b/To-do.xlsx
@@ -2191,8 +2191,8 @@
   <dimension ref="A1:E140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3250,19 +3250,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C139:C140"/>
-    <mergeCell ref="C123:C126"/>
-    <mergeCell ref="C127:C129"/>
-    <mergeCell ref="C130:C132"/>
-    <mergeCell ref="C110:C116"/>
-    <mergeCell ref="C136:C138"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C98:C102"/>
-    <mergeCell ref="C89:C95"/>
-    <mergeCell ref="C73:C78"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C86:C88"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="C2:C14"/>
     <mergeCell ref="C20:C22"/>
@@ -3277,6 +3264,19 @@
     <mergeCell ref="C35:C44"/>
     <mergeCell ref="C49:C53"/>
     <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C89:C95"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C139:C140"/>
+    <mergeCell ref="C123:C126"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="C130:C132"/>
+    <mergeCell ref="C110:C116"/>
+    <mergeCell ref="C136:C138"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="Spring!A1" display="Spring"/>

</xml_diff>